<commit_message>
basic functionality working for word docs and excel files
</commit_message>
<xml_diff>
--- a/FinalProject.2025.08.10/ExampleFiles/TeamMemberFour.xlsx
+++ b/FinalProject.2025.08.10/ExampleFiles/TeamMemberFour.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E.M. Janssen\Documents\GitHub\COMP1112.Python.2025\FinalProject.2025.08.10\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D0F9D9-FC47-4F0D-8186-5988E2B9203A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513AA19D-0570-46DE-B905-9D1B37E6CE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{076963AE-B970-45A8-A1AB-A22BED4A8A9A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{076963AE-B970-45A8-A1AB-A22BED4A8A9A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Program Info" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -556,7 +556,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>